<commit_message>
xldownload for both blockdetails and unitdetails updated
</commit_message>
<xml_diff>
--- a/src/assets/Excel/Demo_Block_Detailstemplate.xlsx
+++ b/src/assets/Excel/Demo_Block_Detailstemplate.xlsx
@@ -1,75 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anusha\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6A5EA4A-B7F4-4F07-9B1E-1629F3918C26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="1968" yWindow="2568" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
   <si>
     <t>Sno</t>
-  </si>
-  <si>
-    <t>BlockName</t>
-  </si>
-  <si>
-    <t>BlockType</t>
-  </si>
-  <si>
-    <t>NumberOfUnits</t>
-  </si>
-  <si>
-    <t>ManagerName</t>
-  </si>
-  <si>
-    <t>ManagerMobileNumber</t>
-  </si>
-  <si>
-    <t>ManagerEmailID</t>
-  </si>
-  <si>
-    <t>FlatRateValue(amount/flat)</t>
-  </si>
-  <si>
-    <t>MaintenanceValue(Rupees/Sqft)</t>
-  </si>
-  <si>
-    <t>InvoiceCreationFrequency</t>
-  </si>
-  <si>
-    <t>InvoiceGenerationDate</t>
-  </si>
-  <si>
-    <t>InvoiceDueDate</t>
-  </si>
-  <si>
-    <t>LatePaymentChargeType</t>
-  </si>
-  <si>
-    <t>LatePaymentCharge</t>
-  </si>
-  <si>
-    <t>StartsFrom</t>
-  </si>
-  <si>
-    <t>Block-A</t>
-  </si>
-  <si>
-    <t>Residential</t>
-  </si>
-  <si>
-    <t>Sam</t>
   </si>
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="12"/>
         <rFont val="Helvetica Neue"/>
@@ -78,30 +36,9 @@
     </r>
   </si>
   <si>
-    <t>Monthly</t>
-  </si>
-  <si>
-    <t>2019/12/31</t>
-  </si>
-  <si>
-    <t>2020/01/05</t>
-  </si>
-  <si>
-    <t>2020/01/10</t>
-  </si>
-  <si>
-    <t>Block-B</t>
-  </si>
-  <si>
-    <t>Commercial</t>
-  </si>
-  <si>
-    <t>John</t>
-  </si>
-  <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="12"/>
         <rFont val="Helvetica Neue"/>
@@ -110,92 +47,78 @@
     </r>
   </si>
   <si>
-    <t>Quarterly</t>
-  </si>
-  <si>
-    <t>2019/12/32</t>
-  </si>
-  <si>
-    <t>quaterly</t>
-  </si>
-  <si>
-    <t>Block-C</t>
-  </si>
-  <si>
-    <t>Residential and Commercial</t>
-  </si>
-  <si>
-    <t>Daniel</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="12"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>daniel@gmail.com</t>
-    </r>
-  </si>
-  <si>
-    <t>Half Yearly</t>
-  </si>
-  <si>
-    <t>2019/12/33</t>
-  </si>
-  <si>
-    <t>Annually</t>
-  </si>
-  <si>
-    <t>Block-D</t>
-  </si>
-  <si>
-    <t>Joy</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="12"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>joy@gmail.com</t>
-    </r>
-  </si>
-  <si>
-    <t>Yearly</t>
-  </si>
-  <si>
-    <t>2019/12/34</t>
+    <t>blocktype</t>
+  </si>
+  <si>
+    <t>units</t>
+  </si>
+  <si>
+    <t>managername</t>
+  </si>
+  <si>
+    <t>managermobileno</t>
+  </si>
+  <si>
+    <t>manageremailid</t>
+  </si>
+  <si>
+    <t>RESIDENTIAL</t>
+  </si>
+  <si>
+    <t>COMMERCIAL</t>
+  </si>
+  <si>
+    <t>BLOCK-A</t>
+  </si>
+  <si>
+    <t>BLOCK-B</t>
+  </si>
+  <si>
+    <t>SAM</t>
+  </si>
+  <si>
+    <t>JPHN</t>
+  </si>
+  <si>
+    <t>SATYA</t>
+  </si>
+  <si>
+    <t>BLOCK-C</t>
+  </si>
+  <si>
+    <t>BLOCK-D</t>
+  </si>
+  <si>
+    <t>BLOCK-E</t>
+  </si>
+  <si>
+    <t>BLOCK-F</t>
+  </si>
+  <si>
+    <t>SILVER</t>
+  </si>
+  <si>
+    <t>ANU</t>
+  </si>
+  <si>
+    <t>DADY</t>
+  </si>
+  <si>
+    <t>blockname</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="13"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <u val="single"/>
+      <u/>
       <sz val="10"/>
       <color indexed="12"/>
       <name val="Helvetica Neue"/>
@@ -255,24 +178,24 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -283,26 +206,85 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffa5a5a5"/>
-      <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ff0000ff"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFA5A5A5"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Blank">
   <a:themeElements>
     <a:clrScheme name="Blank">
       <a:dk1>
@@ -504,7 +486,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -523,7 +505,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -553,7 +535,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -579,7 +561,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -605,7 +587,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -631,7 +613,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -657,7 +639,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -683,7 +665,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -709,7 +691,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -735,7 +717,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -761,7 +743,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -774,9 +756,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -793,7 +781,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -812,7 +800,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -838,7 +826,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -864,7 +852,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -890,7 +878,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -916,7 +904,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -942,7 +930,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -968,7 +956,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -994,7 +982,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1020,7 +1008,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1046,7 +1034,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1059,9 +1047,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1075,7 +1069,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1094,7 +1088,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1124,7 +1118,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1150,7 +1144,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1176,7 +1170,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1202,7 +1196,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1228,7 +1222,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1254,7 +1248,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1280,7 +1274,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1306,7 +1300,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1332,7 +1326,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1345,285 +1339,218 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:IM7"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="15.1" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="15.15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="7.35156" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.6719" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.0781" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.9141" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15.2266" style="1" customWidth="1"/>
-    <col min="6" max="6" width="20.6328" style="1" customWidth="1"/>
-    <col min="7" max="7" width="25.8516" style="1" customWidth="1"/>
-    <col min="8" max="8" width="22.2422" style="1" customWidth="1"/>
-    <col min="9" max="9" width="26.9844" style="1" customWidth="1"/>
-    <col min="10" max="10" width="22.9531" style="1" customWidth="1"/>
-    <col min="11" max="15" width="20.8516" style="1" customWidth="1"/>
-    <col min="16" max="256" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.21875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="20.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="25.6640625" style="1" customWidth="1"/>
+    <col min="8" max="247" width="16.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="32.25" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:7" ht="32.25" customHeight="1">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="2">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s" s="2">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s" s="2">
+      <c r="B1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="2">
+      <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="2">
+      <c r="E1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s" s="2">
+      <c r="F1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s" s="2">
+      <c r="G1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s" s="2">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s" s="2">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s" s="2">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s" s="2">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s" s="2">
-        <v>13</v>
-      </c>
-      <c r="O1" t="s" s="2">
-        <v>14</v>
-      </c>
     </row>
-    <row r="2" ht="20.05" customHeight="1">
+    <row r="2" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="2">
-        <v>15</v>
-      </c>
-      <c r="C2" t="s" s="2">
-        <v>16</v>
+      <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="D2" s="4">
-        <v>50</v>
-      </c>
-      <c r="E2" t="s" s="2">
-        <v>17</v>
+        <v>5</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="F2" s="4">
         <v>9999999999</v>
       </c>
-      <c r="G2" t="s" s="2">
-        <v>18</v>
-      </c>
-      <c r="H2" s="4">
-        <v>3600</v>
-      </c>
-      <c r="I2" s="4">
-        <v>6.5</v>
-      </c>
-      <c r="J2" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="K2" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="L2" t="s" s="2">
-        <v>21</v>
-      </c>
-      <c r="M2" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="N2" s="4">
-        <v>600</v>
-      </c>
-      <c r="O2" t="s" s="2">
-        <v>22</v>
+      <c r="G2" s="2" t="s">
+        <v>1</v>
       </c>
     </row>
-    <row r="3" ht="14.7" customHeight="1">
+    <row r="3" spans="1:7" ht="14.7" customHeight="1">
       <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" t="s" s="2">
-        <v>23</v>
-      </c>
-      <c r="C3" t="s" s="2">
-        <v>24</v>
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="D3" s="4">
-        <v>60</v>
-      </c>
-      <c r="E3" t="s" s="2">
-        <v>25</v>
+        <v>6</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="F3" s="4">
         <v>8888888888</v>
       </c>
-      <c r="G3" t="s" s="2">
-        <v>26</v>
-      </c>
-      <c r="H3" s="4">
-        <v>3600</v>
-      </c>
-      <c r="I3" s="4">
-        <v>6</v>
-      </c>
-      <c r="J3" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="K3" t="s" s="2">
-        <v>28</v>
-      </c>
-      <c r="L3" t="s" s="2">
-        <v>21</v>
-      </c>
-      <c r="M3" t="s" s="2">
-        <v>29</v>
-      </c>
-      <c r="N3" s="4">
-        <v>600</v>
-      </c>
-      <c r="O3" t="s" s="2">
-        <v>22</v>
+      <c r="G3" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="4" ht="14.7" customHeight="1">
-      <c r="A4" s="4">
+    <row r="4" spans="1:7" ht="15.15" customHeight="1">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" t="s" s="2">
-        <v>30</v>
-      </c>
-      <c r="C4" t="s" s="2">
-        <v>31</v>
+      <c r="B4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="D4" s="4">
-        <v>70</v>
-      </c>
-      <c r="E4" t="s" s="2">
-        <v>32</v>
+        <v>4</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="F4" s="4">
         <v>7777777777</v>
       </c>
-      <c r="G4" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="H4" s="4">
-        <v>3600</v>
-      </c>
-      <c r="I4" s="4">
-        <v>6</v>
-      </c>
-      <c r="J4" t="s" s="2">
-        <v>34</v>
-      </c>
-      <c r="K4" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="L4" t="s" s="2">
-        <v>21</v>
-      </c>
-      <c r="M4" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="N4" s="4">
-        <v>600</v>
-      </c>
-      <c r="O4" t="s" s="2">
-        <v>22</v>
+      <c r="G4" s="2" t="s">
+        <v>1</v>
       </c>
     </row>
-    <row r="5" ht="14.7" customHeight="1">
+    <row r="5" spans="1:7" ht="15.15" customHeight="1">
       <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="C5" t="s" s="2">
+      <c r="B5" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="C5" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="D5" s="4">
-        <v>80</v>
-      </c>
-      <c r="E5" t="s" s="2">
-        <v>38</v>
+        <v>3</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="F5" s="4">
         <v>6666666666</v>
       </c>
-      <c r="G5" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="H5" s="4">
-        <v>4600</v>
-      </c>
-      <c r="I5" s="4">
+      <c r="G5" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15.15" customHeight="1">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="4">
+        <v>2</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="4">
+        <v>5555555555</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.15" customHeight="1">
+      <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="J5" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="K5" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="L5" t="s" s="2">
+      <c r="B7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="4">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="M5" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="N5" s="4">
-        <v>600</v>
-      </c>
-      <c r="O5" t="s" s="2">
-        <v>22</v>
+      <c r="F7" s="4">
+        <v>4444444444</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" location="" tooltip="" display="sam007@gmail.com"/>
-    <hyperlink ref="G3" r:id="rId2" location="" tooltip="" display="john@gmail.com"/>
-    <hyperlink ref="G4" r:id="rId3" location="" tooltip="" display="daniel@gmail.com"/>
-    <hyperlink ref="G5" r:id="rId4" location="" tooltip="" display="joy@gmail.com"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{1CD42F79-478E-44FF-A834-CBE0B10AB0FD}"/>
+    <hyperlink ref="G5" r:id="rId4" xr:uid="{4E104BEF-61BD-468C-B28E-39E6915E63EA}"/>
+    <hyperlink ref="G6" r:id="rId5" xr:uid="{2396118F-FF91-4881-8BBA-B1D4D80A76C0}"/>
+    <hyperlink ref="G7" r:id="rId6" xr:uid="{A8EF0301-2CD3-4633-AC62-66D88DC88946}"/>
   </hyperlinks>
-  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Implemented Bulkupload for Unit level including duplicate same as while creating association new UI
</commit_message>
<xml_diff>
--- a/src/assets/Excel/Demo_Block_Detailstemplate.xlsx
+++ b/src/assets/Excel/Demo_Block_Detailstemplate.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anusha\Desktop\New folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anusha\Desktop\blocklevel excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{260D2AE2-085D-4C18-83F4-FA0ADB24A270}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7274AC7D-4585-445B-B097-BF1EE8792D7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1848" yWindow="1848" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2544" yWindow="2544" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,36 +20,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
   <si>
     <t>Sno</t>
   </si>
   <si>
-    <t>BlockName</t>
-  </si>
-  <si>
-    <t>BlockType</t>
-  </si>
-  <si>
-    <t>NumberOfUnits</t>
-  </si>
-  <si>
-    <t>ManagerName</t>
-  </si>
-  <si>
-    <t>ManagerMobileNumber</t>
-  </si>
-  <si>
-    <t>ManagerEmailID</t>
-  </si>
-  <si>
-    <t>Block-A</t>
+    <t>blockname</t>
+  </si>
+  <si>
+    <t>blocktype</t>
+  </si>
+  <si>
+    <t>units</t>
+  </si>
+  <si>
+    <t>managername</t>
+  </si>
+  <si>
+    <t>managermobileno</t>
+  </si>
+  <si>
+    <t>manageremailid</t>
   </si>
   <si>
     <t>Residential</t>
   </si>
   <si>
-    <t>Sam</t>
+    <t>SAM</t>
   </si>
   <si>
     <r>
@@ -63,13 +60,10 @@
     </r>
   </si>
   <si>
-    <t>Block-B</t>
-  </si>
-  <si>
     <t>Commercial</t>
   </si>
   <si>
-    <t>John</t>
+    <t>JPHN</t>
   </si>
   <si>
     <r>
@@ -83,47 +77,37 @@
     </r>
   </si>
   <si>
-    <t>Block-C</t>
-  </si>
-  <si>
     <t>Residential and Commercial</t>
   </si>
   <si>
-    <t>Daniel</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <color indexed="12"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>daniel@gmail.com</t>
-    </r>
-  </si>
-  <si>
-    <t>Block-D</t>
-  </si>
-  <si>
-    <t>Joy</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <color indexed="12"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>joy@gmail.com</t>
-    </r>
-  </si>
-  <si>
-    <t>Block-E</t>
-  </si>
-  <si>
-    <t>satya</t>
+    <t>SATYA</t>
+  </si>
+  <si>
+    <t>SILVER</t>
+  </si>
+  <si>
+    <t>ANU</t>
+  </si>
+  <si>
+    <t>DADY</t>
+  </si>
+  <si>
+    <t>BLOCK3</t>
+  </si>
+  <si>
+    <t>BLOCK4</t>
+  </si>
+  <si>
+    <t>BLOCK5</t>
+  </si>
+  <si>
+    <t>BLOCK6</t>
+  </si>
+  <si>
+    <t>BLOCK1</t>
+  </si>
+  <si>
+    <t>BLOCK2</t>
   </si>
 </sst>
 </file>
@@ -157,7 +141,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -195,13 +179,100 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -215,6 +286,33 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1380,22 +1478,22 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IN6"/>
+  <dimension ref="A1:IV10"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="15.15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="7.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="19.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.21875" style="1" customWidth="1"/>
     <col min="4" max="4" width="13.88671875" style="1" customWidth="1"/>
     <col min="5" max="5" width="15.21875" style="1" customWidth="1"/>
     <col min="6" max="6" width="20.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="25.88671875" style="1" customWidth="1"/>
-    <col min="8" max="248" width="16.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="25.6640625" style="1" customWidth="1"/>
+    <col min="8" max="256" width="16.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="32.25" customHeight="1">
@@ -1426,22 +1524,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="4">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="D2" s="4">
-        <v>5</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="F2" s="4">
         <v>9886819118</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="14.7" customHeight="1">
@@ -1449,48 +1547,48 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="4">
+        <v>4</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="4">
-        <v>6</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="F3" s="4">
         <v>9886819118</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.15" customHeight="1">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="4">
+        <v>4</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="14.7" customHeight="1">
-      <c r="A4" s="4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="4">
-        <v>7</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="F4" s="4">
         <v>9886819118</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="14.7" customHeight="1">
+    <row r="5" spans="1:7" ht="15.15" customHeight="1">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -1498,51 +1596,107 @@
         <v>19</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5" s="4">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F5" s="4">
         <v>9886819118</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="14.7" customHeight="1">
-      <c r="A6" s="4">
+    <row r="6" spans="1:7" ht="15.15" customHeight="1">
+      <c r="A6" s="3">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D6" s="4">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="F6" s="4">
         <v>9886819118</v>
       </c>
       <c r="G6" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.15" customHeight="1">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="C7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="4">
+        <v>4</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="4">
+        <v>9886819118</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="14.7" customHeight="1">
+      <c r="A8" s="5"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="7"/>
+    </row>
+    <row r="9" spans="1:7" ht="14.7" customHeight="1">
+      <c r="A9" s="8"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="10"/>
+    </row>
+    <row r="10" spans="1:7" ht="14.7" customHeight="1">
+      <c r="A10" s="11"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="13"/>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C8" xr:uid="{14D60CE0-C804-42C5-9470-32C762C64AA8}">
+      <formula1>"Residential,Commercial,Residential and Commercial"</formula1>
+    </dataValidation>
+  </dataValidations>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="G3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="G4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
     <hyperlink ref="G5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="G6" r:id="rId5" xr:uid="{73E4A142-B9FE-4BF2-B544-A1C3C035C808}"/>
+    <hyperlink ref="G6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="G7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
   <pageSetup orientation="portrait"/>

</xml_diff>